<commit_message>
Fix system use case description
</commit_message>
<xml_diff>
--- a/Design/API.xlsx
+++ b/Design/API.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>STT</t>
   </si>
@@ -302,6 +302,32 @@
   </si>
   <si>
     <t>File {file_name}.jpg</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>[POST]book/update_author</t>
+  </si>
+  <si>
+    <t>{
+     "id": 7,
+     "name": "Nam Cao",
+     "currentUserID": 1
+}</t>
+  </si>
+  <si>
+    <t>{
+    "result": true,
+    "message": "Cập nhật thành công",
+    "data": {
+        "id": 7,
+        "name": "Nam Cao",
+        "updatedDate": "15-08-2020",
+        "updatedAccount": "Võ Thanh Hiếu",
+        "updatedAccountID": 1
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -345,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,11 +406,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -675,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H184"/>
+  <dimension ref="A3:H185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,25 +722,25 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
@@ -741,13 +770,13 @@
       <c r="D7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="4"/>
@@ -763,11 +792,11 @@
       <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -781,11 +810,11 @@
       <c r="D9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -799,11 +828,11 @@
       <c r="D10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -817,11 +846,11 @@
       <c r="D11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -835,11 +864,11 @@
       <c r="D12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -853,11 +882,11 @@
       <c r="D13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -875,7 +904,7 @@
         <v>36</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="4"/>
@@ -893,7 +922,7 @@
         <v>38</v>
       </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1022,65 +1051,73 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>11</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>54</v>
-      </c>
+    <row r="22" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="4" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="G22" s="5" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>12</v>
-      </c>
-      <c r="B23" s="13"/>
+        <v>11</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="C23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>12</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>13</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
@@ -1092,7 +1129,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
@@ -1104,7 +1141,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
@@ -1116,7 +1153,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
@@ -1128,7 +1165,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -1138,9 +1175,9 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
@@ -1150,9 +1187,9 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
@@ -1164,7 +1201,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -1176,7 +1213,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
@@ -1188,7 +1225,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
@@ -1200,7 +1237,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -1212,7 +1249,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
@@ -1224,7 +1261,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
@@ -1236,7 +1273,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -1248,7 +1285,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -1260,7 +1297,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -1272,7 +1309,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
@@ -1284,7 +1321,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
@@ -1296,7 +1333,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>
@@ -1308,7 +1345,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
@@ -1320,7 +1357,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
@@ -1332,7 +1369,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
@@ -1344,7 +1381,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
@@ -1356,7 +1393,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
@@ -1368,7 +1405,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
@@ -1380,7 +1417,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
@@ -1392,7 +1429,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
@@ -1404,7 +1441,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
@@ -1416,7 +1453,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
@@ -1428,7 +1465,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
@@ -1440,7 +1477,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
@@ -1452,7 +1489,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
@@ -1464,7 +1501,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
@@ -1476,7 +1513,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="4"/>
@@ -1488,7 +1525,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
@@ -1500,7 +1537,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
@@ -1512,7 +1549,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="4"/>
@@ -1524,7 +1561,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
@@ -1536,7 +1573,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="4"/>
@@ -1548,7 +1585,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
@@ -1560,7 +1597,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
@@ -1572,7 +1609,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4"/>
@@ -1584,7 +1621,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
@@ -1596,7 +1633,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4"/>
@@ -1608,7 +1645,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="4"/>
@@ -1620,7 +1657,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="4"/>
@@ -1632,7 +1669,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="4"/>
@@ -1644,7 +1681,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
@@ -1656,7 +1693,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="4"/>
@@ -1668,7 +1705,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4"/>
@@ -1680,7 +1717,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
@@ -1692,7 +1729,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
@@ -1704,7 +1741,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
@@ -1716,7 +1753,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
@@ -1728,7 +1765,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
@@ -1740,7 +1777,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
@@ -1752,7 +1789,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4"/>
@@ -1764,7 +1801,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
@@ -1776,7 +1813,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4"/>
@@ -1788,7 +1825,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="4"/>
@@ -1800,7 +1837,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
@@ -1812,7 +1849,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4"/>
@@ -1824,7 +1861,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4"/>
@@ -1836,7 +1873,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="4"/>
@@ -1848,7 +1885,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
@@ -1860,7 +1897,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="4"/>
@@ -1872,7 +1909,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="4"/>
@@ -1884,7 +1921,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="4"/>
@@ -1896,7 +1933,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="4"/>
@@ -1908,7 +1945,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="4"/>
@@ -1920,7 +1957,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="4"/>
@@ -1932,7 +1969,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="4"/>
@@ -1944,7 +1981,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="4"/>
@@ -1956,7 +1993,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="4"/>
@@ -1968,7 +2005,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="4"/>
@@ -1980,7 +2017,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="4"/>
@@ -1992,7 +2029,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="4"/>
@@ -2004,7 +2041,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="4"/>
@@ -2016,7 +2053,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="4"/>
@@ -2028,7 +2065,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="4"/>
@@ -2040,7 +2077,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="4"/>
@@ -2052,7 +2089,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="4"/>
@@ -2064,7 +2101,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="4"/>
@@ -2076,7 +2113,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="4"/>
@@ -2088,7 +2125,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="4"/>
@@ -2100,7 +2137,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="4"/>
@@ -2112,7 +2149,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="4"/>
@@ -2124,7 +2161,7 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="4"/>
@@ -2136,7 +2173,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="4"/>
@@ -2148,7 +2185,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="4"/>
@@ -2160,7 +2197,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="4"/>
@@ -2172,7 +2209,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="4"/>
@@ -2184,7 +2221,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B117" s="3"/>
       <c r="C117" s="4"/>
@@ -2196,7 +2233,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" s="4"/>
@@ -2208,7 +2245,7 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B119" s="3"/>
       <c r="C119" s="4"/>
@@ -2220,7 +2257,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B120" s="3"/>
       <c r="C120" s="4"/>
@@ -2232,7 +2269,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="4"/>
@@ -2244,7 +2281,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="4"/>
@@ -2256,7 +2293,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B123" s="3"/>
       <c r="C123" s="4"/>
@@ -2268,7 +2305,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="4"/>
@@ -2280,7 +2317,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="4"/>
@@ -2292,7 +2329,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="4"/>
@@ -2304,7 +2341,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="4"/>
@@ -2316,7 +2353,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="4"/>
@@ -2328,7 +2365,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B129" s="3"/>
       <c r="C129" s="4"/>
@@ -2340,7 +2377,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="4"/>
@@ -2352,7 +2389,7 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B131" s="3"/>
       <c r="C131" s="4"/>
@@ -2364,7 +2401,7 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B132" s="3"/>
       <c r="C132" s="4"/>
@@ -2376,7 +2413,7 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B133" s="3"/>
       <c r="C133" s="4"/>
@@ -2388,7 +2425,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B134" s="3"/>
       <c r="C134" s="4"/>
@@ -2400,7 +2437,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="4"/>
@@ -2412,7 +2449,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="4"/>
@@ -2424,7 +2461,7 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="4"/>
@@ -2436,7 +2473,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B138" s="3"/>
       <c r="C138" s="4"/>
@@ -2448,7 +2485,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B139" s="3"/>
       <c r="C139" s="4"/>
@@ -2460,7 +2497,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B140" s="3"/>
       <c r="C140" s="4"/>
@@ -2472,7 +2509,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B141" s="3"/>
       <c r="C141" s="4"/>
@@ -2484,7 +2521,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B142" s="3"/>
       <c r="C142" s="4"/>
@@ -2496,7 +2533,7 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B143" s="3"/>
       <c r="C143" s="4"/>
@@ -2508,7 +2545,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B144" s="3"/>
       <c r="C144" s="4"/>
@@ -2520,7 +2557,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B145" s="3"/>
       <c r="C145" s="4"/>
@@ -2532,7 +2569,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B146" s="3"/>
       <c r="C146" s="4"/>
@@ -2544,7 +2581,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B147" s="3"/>
       <c r="C147" s="4"/>
@@ -2556,7 +2593,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B148" s="3"/>
       <c r="C148" s="4"/>
@@ -2568,7 +2605,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B149" s="3"/>
       <c r="C149" s="4"/>
@@ -2580,7 +2617,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B150" s="3"/>
       <c r="C150" s="4"/>
@@ -2592,7 +2629,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B151" s="3"/>
       <c r="C151" s="4"/>
@@ -2604,7 +2641,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B152" s="3"/>
       <c r="C152" s="4"/>
@@ -2616,7 +2653,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B153" s="3"/>
       <c r="C153" s="4"/>
@@ -2628,7 +2665,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B154" s="3"/>
       <c r="C154" s="4"/>
@@ -2640,7 +2677,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B155" s="3"/>
       <c r="C155" s="4"/>
@@ -2652,7 +2689,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B156" s="3"/>
       <c r="C156" s="4"/>
@@ -2664,7 +2701,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B157" s="3"/>
       <c r="C157" s="4"/>
@@ -2676,7 +2713,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="4"/>
@@ -2688,7 +2725,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="4"/>
@@ -2700,7 +2737,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="4"/>
@@ -2712,7 +2749,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="4"/>
@@ -2724,7 +2761,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B162" s="3"/>
       <c r="C162" s="4"/>
@@ -2736,7 +2773,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B163" s="3"/>
       <c r="C163" s="4"/>
@@ -2748,7 +2785,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B164" s="3"/>
       <c r="C164" s="4"/>
@@ -2760,7 +2797,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="4"/>
@@ -2772,7 +2809,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="4"/>
@@ -2784,7 +2821,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B167" s="3"/>
       <c r="C167" s="4"/>
@@ -2796,7 +2833,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="4"/>
@@ -2808,7 +2845,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B169" s="3"/>
       <c r="C169" s="4"/>
@@ -2820,7 +2857,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B170" s="3"/>
       <c r="C170" s="4"/>
@@ -2832,7 +2869,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B171" s="3"/>
       <c r="C171" s="4"/>
@@ -2844,7 +2881,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B172" s="3"/>
       <c r="C172" s="4"/>
@@ -2856,7 +2893,7 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B173" s="3"/>
       <c r="C173" s="4"/>
@@ -2868,7 +2905,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B174" s="3"/>
       <c r="C174" s="4"/>
@@ -2880,7 +2917,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B175" s="3"/>
       <c r="C175" s="4"/>
@@ -2892,7 +2929,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B176" s="3"/>
       <c r="C176" s="4"/>
@@ -2904,7 +2941,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B177" s="3"/>
       <c r="C177" s="4"/>
@@ -2916,7 +2953,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B178" s="3"/>
       <c r="C178" s="4"/>
@@ -2928,7 +2965,7 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B179" s="3"/>
       <c r="C179" s="4"/>
@@ -2940,7 +2977,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B180" s="3"/>
       <c r="C180" s="4"/>
@@ -2952,7 +2989,7 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B181" s="3"/>
       <c r="C181" s="4"/>
@@ -2964,7 +3001,7 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B182" s="3"/>
       <c r="C182" s="4"/>
@@ -2976,7 +3013,7 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B183" s="3"/>
       <c r="C183" s="4"/>
@@ -2988,7 +3025,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B184" s="3"/>
       <c r="C184" s="4"/>
@@ -2998,9 +3035,21 @@
       <c r="G184" s="4"/>
       <c r="H184" s="4"/>
     </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="3">
+        <v>173</v>
+      </c>
+      <c r="B185" s="3"/>
+      <c r="C185" s="4"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="4"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="4"/>
+      <c r="H185" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A3:H3"/>

</xml_diff>